<commit_message>
Query improvements and percentage calculation method updates
</commit_message>
<xml_diff>
--- a/server/data/queries/Impact graph type.xlsx
+++ b/server/data/queries/Impact graph type.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cyardimci/Documents/WAAT/Impact/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cyardimci/Projects/WAAT/Impact/impact/server/data/queries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048418B7-ABCA-B74D-92DC-940643C48F16}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6ECE8C-52AD-6146-8B0B-402C3C84962C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="375">
   <si>
     <t>Database</t>
   </si>
@@ -1170,9 +1170,6 @@
   </si>
   <si>
     <t>Temporarily calculated %, check with Serkan for d3</t>
-  </si>
-  <si>
-    <t>Should be the average of indexes ?</t>
   </si>
   <si>
     <t>Should we count unanswered for overall calculation</t>
@@ -1262,7 +1259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1286,11 +1283,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1302,6 +1295,11 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1390,6 +1388,60 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{611EF349-32C4-9E49-A138-EB593AFF88F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BED048E-0E78-DA4E-87AA-DBC6917A6998}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1730,9 +1782,9 @@
   </sheetPr>
   <dimension ref="A1:AA51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1740,7 +1792,7 @@
     <col min="1" max="1" width="9.5" customWidth="1"/>
     <col min="2" max="2" width="4.5" customWidth="1"/>
     <col min="3" max="3" width="38.83203125" customWidth="1"/>
-    <col min="4" max="4" width="36" style="16" customWidth="1"/>
+    <col min="4" max="4" width="55.33203125" style="16" customWidth="1"/>
     <col min="5" max="5" width="20.5" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
     <col min="7" max="7" width="58.83203125" customWidth="1"/>
@@ -1758,7 +1810,7 @@
       <c r="C1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>364</v>
       </c>
       <c r="E1" s="5" t="s">
@@ -1807,7 +1859,7 @@
       <c r="C2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="22"/>
+      <c r="D2" s="20"/>
       <c r="E2" s="7" t="s">
         <v>49</v>
       </c>
@@ -1835,7 +1887,7 @@
       <c r="C3" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="22"/>
+      <c r="D3" s="20"/>
       <c r="E3" s="7" t="s">
         <v>58</v>
       </c>
@@ -1865,14 +1917,14 @@
       <c r="C4" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="22"/>
+      <c r="D4" s="20"/>
       <c r="E4" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="G4" s="18"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="8"/>
       <c r="I4" s="2" t="s">
         <v>31</v>
@@ -1891,7 +1943,7 @@
       <c r="C5" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="22"/>
+      <c r="D5" s="20"/>
       <c r="E5" s="7" t="s">
         <v>70</v>
       </c>
@@ -1917,14 +1969,14 @@
       <c r="C6" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D6" s="22"/>
+      <c r="D6" s="20"/>
       <c r="E6" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="G6" s="18"/>
+      <c r="G6" s="25"/>
       <c r="H6" s="7" t="s">
         <v>77</v>
       </c>
@@ -1945,14 +1997,14 @@
       <c r="C7" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="22"/>
+      <c r="D7" s="20"/>
       <c r="E7" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="G7" s="18"/>
+      <c r="G7" s="25"/>
       <c r="H7" s="7" t="s">
         <v>77</v>
       </c>
@@ -1973,17 +2025,17 @@
       <c r="C8" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="22"/>
+      <c r="D8" s="20"/>
       <c r="E8" s="7" t="s">
         <v>58</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="H8" s="18"/>
+      <c r="H8" s="25"/>
       <c r="I8" s="2" t="s">
         <v>88</v>
       </c>
@@ -1998,12 +2050,10 @@
       <c r="B9" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="23" t="s">
-        <v>372</v>
-      </c>
+      <c r="D9" s="21"/>
       <c r="E9" s="7" t="s">
         <v>70</v>
       </c>
@@ -2033,7 +2083,7 @@
       <c r="C10" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="D10" s="22"/>
+      <c r="D10" s="20"/>
       <c r="E10" s="7" t="s">
         <v>97</v>
       </c>
@@ -2063,14 +2113,14 @@
       <c r="C11" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="D11" s="22"/>
+      <c r="D11" s="20"/>
       <c r="E11" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="G11" s="18"/>
+      <c r="G11" s="25"/>
       <c r="H11" s="8"/>
       <c r="I11" s="2" t="s">
         <v>103</v>
@@ -2089,14 +2139,14 @@
       <c r="C12" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="D12" s="22"/>
+      <c r="D12" s="20"/>
       <c r="E12" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="G12" s="18"/>
+      <c r="G12" s="25"/>
       <c r="H12" s="8"/>
       <c r="I12" s="2" t="s">
         <v>109</v>
@@ -2115,7 +2165,7 @@
       <c r="C13" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="D13" s="22"/>
+      <c r="D13" s="20"/>
       <c r="E13" s="7" t="s">
         <v>70</v>
       </c>
@@ -2145,17 +2195,17 @@
       <c r="C14" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="D14" s="22"/>
+      <c r="D14" s="20"/>
       <c r="E14" s="7" t="s">
         <v>58</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="H14" s="18"/>
+      <c r="H14" s="25"/>
       <c r="I14" s="2" t="s">
         <v>120</v>
       </c>
@@ -2173,16 +2223,16 @@
       <c r="C15" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D15" s="23" t="s">
-        <v>373</v>
+      <c r="D15" s="21" t="s">
+        <v>372</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="G15" s="18"/>
+      <c r="G15" s="25"/>
       <c r="H15" s="7" t="s">
         <v>125</v>
       </c>
@@ -2203,14 +2253,14 @@
       <c r="C16" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="D16" s="22"/>
+      <c r="D16" s="20"/>
       <c r="E16" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="F16" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="G16" s="18"/>
+      <c r="G16" s="25"/>
       <c r="H16" s="8"/>
       <c r="I16" s="2" t="s">
         <v>130</v>
@@ -2229,7 +2279,7 @@
       <c r="C17" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="D17" s="22"/>
+      <c r="D17" s="20"/>
       <c r="E17" s="7" t="s">
         <v>107</v>
       </c>
@@ -2255,14 +2305,14 @@
       <c r="C18" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D18" s="22"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F18" s="19" t="s">
+      <c r="F18" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="G18" s="18"/>
+      <c r="G18" s="25"/>
       <c r="H18" s="8"/>
       <c r="I18" s="2" t="s">
         <v>138</v>
@@ -2281,14 +2331,14 @@
       <c r="C19" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="D19" s="22"/>
+      <c r="D19" s="20"/>
       <c r="E19" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F19" s="19" t="s">
+      <c r="F19" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="G19" s="18"/>
+      <c r="G19" s="25"/>
       <c r="H19" s="8"/>
       <c r="I19" s="2" t="s">
         <v>144</v>
@@ -2307,14 +2357,14 @@
       <c r="C20" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="D20" s="22"/>
+      <c r="D20" s="20"/>
       <c r="E20" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="F20" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="G20" s="18"/>
+      <c r="G20" s="25"/>
       <c r="H20" s="8"/>
       <c r="I20" s="2" t="s">
         <v>147</v>
@@ -2333,14 +2383,14 @@
       <c r="C21" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="D21" s="22"/>
+      <c r="D21" s="20"/>
       <c r="E21" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F21" s="19" t="s">
+      <c r="F21" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="G21" s="18"/>
+      <c r="G21" s="25"/>
       <c r="H21" s="8"/>
       <c r="I21" s="2" t="s">
         <v>151</v>
@@ -2359,14 +2409,14 @@
       <c r="C22" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="D22" s="22"/>
+      <c r="D22" s="20"/>
       <c r="E22" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F22" s="19" t="s">
+      <c r="F22" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="G22" s="18"/>
+      <c r="G22" s="25"/>
       <c r="H22" s="7" t="s">
         <v>77</v>
       </c>
@@ -2387,8 +2437,8 @@
       <c r="C23" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="D23" s="23" t="s">
-        <v>374</v>
+      <c r="D23" s="21" t="s">
+        <v>373</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>158</v>
@@ -2396,10 +2446,10 @@
       <c r="F23" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="G23" s="24" t="s">
         <v>160</v>
       </c>
-      <c r="H23" s="18"/>
+      <c r="H23" s="25"/>
       <c r="I23" s="2" t="s">
         <v>161</v>
       </c>
@@ -2417,8 +2467,8 @@
       <c r="C24" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="D24" s="23" t="s">
-        <v>375</v>
+      <c r="D24" s="21" t="s">
+        <v>374</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>58</v>
@@ -2449,14 +2499,14 @@
       <c r="C25" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="D25" s="22"/>
+      <c r="D25" s="20"/>
       <c r="E25" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F25" s="19" t="s">
+      <c r="F25" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="G25" s="18"/>
+      <c r="G25" s="25"/>
       <c r="H25" s="7" t="s">
         <v>94</v>
       </c>
@@ -2477,16 +2527,16 @@
       <c r="C26" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="D26" s="23" t="s">
+      <c r="D26" s="21" t="s">
         <v>368</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F26" s="19" t="s">
+      <c r="F26" s="24" t="s">
         <v>170</v>
       </c>
-      <c r="G26" s="18"/>
+      <c r="G26" s="25"/>
       <c r="H26" s="7" t="s">
         <v>94</v>
       </c>
@@ -2507,7 +2557,7 @@
       <c r="C27" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="D27" s="22"/>
+      <c r="D27" s="20"/>
       <c r="E27" s="7" t="s">
         <v>65</v>
       </c>
@@ -2535,7 +2585,7 @@
       <c r="C28" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="D28" s="22"/>
+      <c r="D28" s="20"/>
       <c r="E28" s="7" t="s">
         <v>65</v>
       </c>
@@ -2563,14 +2613,14 @@
       <c r="C29" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="D29" s="22"/>
+      <c r="D29" s="20"/>
       <c r="E29" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F29" s="19" t="s">
+      <c r="F29" s="24" t="s">
         <v>180</v>
       </c>
-      <c r="G29" s="18"/>
+      <c r="G29" s="25"/>
       <c r="H29" s="7" t="s">
         <v>94</v>
       </c>
@@ -2591,7 +2641,7 @@
       <c r="C30" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="D30" s="22"/>
+      <c r="D30" s="20"/>
       <c r="E30" s="7" t="s">
         <v>70</v>
       </c>
@@ -2619,7 +2669,7 @@
       <c r="C31" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="D31" s="22"/>
+      <c r="D31" s="20"/>
       <c r="E31" s="7" t="s">
         <v>70</v>
       </c>
@@ -2647,7 +2697,7 @@
       <c r="C32" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="D32" s="22"/>
+      <c r="D32" s="20"/>
       <c r="E32" s="7" t="s">
         <v>70</v>
       </c>
@@ -2675,7 +2725,7 @@
       <c r="C33" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="D33" s="22"/>
+      <c r="D33" s="20"/>
       <c r="E33" s="7" t="s">
         <v>65</v>
       </c>
@@ -2701,7 +2751,7 @@
       <c r="C34" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="D34" s="22"/>
+      <c r="D34" s="20"/>
       <c r="E34" s="7" t="s">
         <v>107</v>
       </c>
@@ -2727,7 +2777,7 @@
       <c r="C35" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="D35" s="24" t="s">
+      <c r="D35" s="22" t="s">
         <v>365</v>
       </c>
       <c r="E35" s="7" t="s">
@@ -2757,7 +2807,7 @@
       <c r="C36" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="D36" s="25" t="s">
+      <c r="D36" s="23" t="s">
         <v>366</v>
       </c>
       <c r="E36" s="7" t="s">
@@ -2787,7 +2837,7 @@
       <c r="C37" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="D37" s="23" t="s">
+      <c r="D37" s="21" t="s">
         <v>367</v>
       </c>
       <c r="E37" s="7" t="s">
@@ -2819,7 +2869,7 @@
       <c r="C38" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D38" s="23" t="s">
+      <c r="D38" s="21" t="s">
         <v>367</v>
       </c>
       <c r="E38" s="7" t="s">
@@ -2851,7 +2901,7 @@
       <c r="C39" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="D39" s="22"/>
+      <c r="D39" s="20"/>
       <c r="E39" s="7" t="s">
         <v>58</v>
       </c>
@@ -2881,7 +2931,7 @@
       <c r="C40" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="D40" s="22"/>
+      <c r="D40" s="20"/>
       <c r="E40" s="7" t="s">
         <v>65</v>
       </c>
@@ -2907,14 +2957,14 @@
       <c r="C41" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="D41" s="22"/>
+      <c r="D41" s="20"/>
       <c r="E41" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F41" s="17" t="s">
+      <c r="F41" s="26" t="s">
         <v>227</v>
       </c>
-      <c r="G41" s="18"/>
+      <c r="G41" s="25"/>
       <c r="H41" s="9" t="s">
         <v>77</v>
       </c>
@@ -2935,14 +2985,14 @@
       <c r="C42" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="D42" s="22"/>
+      <c r="D42" s="20"/>
       <c r="E42" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F42" s="17" t="s">
+      <c r="F42" s="26" t="s">
         <v>236</v>
       </c>
-      <c r="G42" s="18"/>
+      <c r="G42" s="25"/>
       <c r="H42" s="8"/>
       <c r="I42" s="3" t="s">
         <v>240</v>
@@ -2961,15 +3011,15 @@
       <c r="C43" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="D43" s="22"/>
+      <c r="D43" s="20"/>
       <c r="E43" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F43" s="17" t="s">
+      <c r="F43" s="26" t="s">
         <v>247</v>
       </c>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="25"/>
       <c r="I43" s="2" t="s">
         <v>247</v>
       </c>
@@ -2987,15 +3037,15 @@
       <c r="C44" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="D44" s="22"/>
+      <c r="D44" s="20"/>
       <c r="E44" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F44" s="17" t="s">
+      <c r="F44" s="26" t="s">
         <v>251</v>
       </c>
-      <c r="G44" s="18"/>
-      <c r="H44" s="18"/>
+      <c r="G44" s="25"/>
+      <c r="H44" s="25"/>
       <c r="I44" s="2" t="s">
         <v>252</v>
       </c>
@@ -3013,17 +3063,17 @@
       <c r="C45" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="D45" s="22"/>
+      <c r="D45" s="20"/>
       <c r="E45" s="7" t="s">
         <v>70</v>
       </c>
       <c r="F45" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="G45" s="17" t="s">
+      <c r="G45" s="26" t="s">
         <v>259</v>
       </c>
-      <c r="H45" s="18"/>
+      <c r="H45" s="25"/>
       <c r="I45" s="2" t="s">
         <v>25</v>
       </c>
@@ -3041,17 +3091,17 @@
       <c r="C46" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="D46" s="22"/>
+      <c r="D46" s="20"/>
       <c r="E46" s="7" t="s">
         <v>58</v>
       </c>
       <c r="F46" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="G46" s="17" t="s">
+      <c r="G46" s="26" t="s">
         <v>259</v>
       </c>
-      <c r="H46" s="18"/>
+      <c r="H46" s="25"/>
       <c r="I46" s="2" t="s">
         <v>27</v>
       </c>
@@ -3069,7 +3119,7 @@
       <c r="C47" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="D47" s="23" t="s">
+      <c r="D47" s="21" t="s">
         <v>369</v>
       </c>
       <c r="E47" s="7" t="s">
@@ -3101,7 +3151,7 @@
       <c r="C48" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="D48" s="24" t="s">
+      <c r="D48" s="22" t="s">
         <v>370</v>
       </c>
       <c r="E48" s="7" t="s">
@@ -3110,11 +3160,11 @@
       <c r="F48" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="G48" s="17" t="s">
+      <c r="G48" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="H48" s="18"/>
-      <c r="I48" s="20" t="s">
+      <c r="H48" s="25"/>
+      <c r="I48" s="18" t="s">
         <v>287</v>
       </c>
       <c r="J48" s="2" t="s">
@@ -3131,7 +3181,7 @@
       <c r="C49" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="D49" s="23" t="s">
+      <c r="D49" s="21" t="s">
         <v>371</v>
       </c>
       <c r="E49" s="7" t="s">
@@ -3161,15 +3211,15 @@
       <c r="C50" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="D50" s="22"/>
+      <c r="D50" s="20"/>
       <c r="E50" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F50" s="17" t="s">
+      <c r="F50" s="26" t="s">
         <v>294</v>
       </c>
-      <c r="G50" s="18"/>
-      <c r="H50" s="18"/>
+      <c r="G50" s="25"/>
+      <c r="H50" s="25"/>
       <c r="I50" s="2" t="s">
         <v>295</v>
       </c>
@@ -3187,14 +3237,14 @@
       <c r="C51" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="D51" s="22"/>
+      <c r="D51" s="20"/>
       <c r="E51" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F51" s="17" t="s">
+      <c r="F51" s="26" t="s">
         <v>291</v>
       </c>
-      <c r="G51" s="18"/>
+      <c r="G51" s="25"/>
       <c r="H51" s="8"/>
       <c r="I51" s="2" t="s">
         <v>297</v>
@@ -3206,6 +3256,18 @@
   </sheetData>
   <autoFilter ref="A1:H51" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="27">
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="F43:H43"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F26:G26"/>
     <mergeCell ref="F22:G22"/>
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="F6:G6"/>
@@ -3221,18 +3283,6 @@
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="F43:H43"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G46:H46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>